<commit_message>
Extract PNCC from PDF. Fix typo (not mine!) in KCDC mayor's name
</commit_message>
<xml_diff>
--- a/sources/2019/kcdc_mayor.xlsx
+++ b/sources/2019/kcdc_mayor.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Final results\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidFriggens\OneDrive - Infometrics\skunkworks\stv19\iterations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_5014B33C26089E73CB4DCEE435BA4352A8D4A5A1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2CE8098-CA23-4A09-8B0D-C6218DD9BEBF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12330"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,8 +20,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="STV_Result_Election_KapitiCoastDistrictCouncil_Issue_Mayor16_10_2019121357PM_N" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="STV_Result_Election_KapitiCoastDistrictCouncil_Issue_Mayor16_10_2019121357PM_N" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Final results\STV_Result_Election_KapitiCoastDistrictCouncil_Issue_Mayor16_10_2019121357PM_N.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -95,9 +96,6 @@
     <t>Elliott Jackie</t>
   </si>
   <si>
-    <t>Guruanthan K (Guru)</t>
-  </si>
-  <si>
     <t>Halliday Martin</t>
   </si>
   <si>
@@ -108,12 +106,15 @@
   </si>
   <si>
     <t>elected</t>
+  </si>
+  <si>
+    <t>Gurunathan K (Guru)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,52 +224,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O13" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:O13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O13" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:O13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" uniqueName="container-id" name="container-id">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="container-id" name="container-id">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/@container-id" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="calculator-version" name="calculator-version">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="calculator-version" name="calculator-version">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/@calculator-version" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="resource-id" name="resource-id">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="resource-id" name="resource-id">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns1:input-container/@resource-id" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="4" uniqueName="name" name="name">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="name" name="name">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns1:input-container/@name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" uniqueName="location" name="location">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="location" name="location">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns1:input-container/@location" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="number" name="number">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="number" name="number">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/@number" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="quota" name="quota">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="quota" name="quota">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/@quota" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ntv" name="ntv">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ntv" name="ntv">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/@ntv" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="surplus" name="surplus">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="surplus" name="surplus">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/@surplus" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="id" name="id">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="id" name="id">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@id" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="11" uniqueName="vote-count" name="vote-count">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" uniqueName="vote-count" name="vote-count">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@vote-count" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="12" uniqueName="keep-value" name="keep-value">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="keep-value" name="keep-value">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@keep-value" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="13" uniqueName="surplus" name="surplus2">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="surplus" name="surplus2">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@surplus" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="14" uniqueName="random" name="random">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="random" name="random">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@random" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="15" uniqueName="status" name="status">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="status" name="status">
       <xmlColumnPr mapId="1" xpath="/ns1:output-container/ns2:iterations/ns2:iteration/ns2:candidate/@status" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -538,31 +539,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -653,10 +654,10 @@
         <v>5229</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -700,10 +701,10 @@
         <v>3812</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -732,7 +733,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K4">
         <v>7879</v>
@@ -747,10 +748,10 @@
         <v>9028</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -779,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5">
         <v>2058</v>
@@ -794,10 +795,10 @@
         <v>2610</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -841,10 +842,10 @@
         <v>4771</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -888,10 +889,10 @@
         <v>6188</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -920,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K8">
         <v>8253</v>
@@ -935,10 +936,10 @@
         <v>972</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -967,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -982,10 +983,10 @@
         <v>7390</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1029,10 +1030,10 @@
         <v>5229</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1076,10 +1077,10 @@
         <v>3812</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>485</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K12">
         <v>9029</v>
@@ -1123,10 +1124,10 @@
         <v>9028</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>485</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1170,7 +1171,7 @@
         <v>2610</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>